<commit_message>
Added excel data source code where ever it is possible
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santh\Desktop\Ecommerce Automation\Selenium\EcommercePractise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD4BDBC6-843B-4308-BED7-B6A187FCE6EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7BEF483-0202-4CB8-A442-202AA970200E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t>santhoshsai4517@gmail.com</t>
   </si>
@@ -46,6 +46,24 @@
   </si>
   <si>
     <t>jan.feil@yahoo.com</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>tony.tillman@hotmail.com</t>
+  </si>
+  <si>
+    <t>5ok0nflrcj5</t>
+  </si>
+  <si>
+    <t>genna.keebler@gmail.com</t>
+  </si>
+  <si>
+    <t>af1ys6r4mb7i0</t>
+  </si>
+  <si>
+    <t>nerissa.hagenes@yahoo.com</t>
   </si>
 </sst>
 </file>
@@ -384,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B7" sqref="A6:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -421,7 +439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s" s="0">
         <v>5</v>
       </c>
@@ -429,11 +447,35 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s" s="0">
         <v>6</v>
       </c>
       <c r="B5" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s" s="0">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated selenium version to use latest chrome browser and completed E@E UI validations
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santh\Desktop\Ecommerce Automation\Selenium\EcommercePractise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7BEF483-0202-4CB8-A442-202AA970200E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EECE3C-34CB-40B7-A348-E8DC8CD664E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="58">
   <si>
     <t>santhoshsai4517@gmail.com</t>
   </si>
@@ -60,10 +60,145 @@
     <t>genna.keebler@gmail.com</t>
   </si>
   <si>
-    <t>af1ys6r4mb7i0</t>
-  </si>
-  <si>
     <t>nerissa.hagenes@yahoo.com</t>
+  </si>
+  <si>
+    <t>derek.monahan@hotmail.com</t>
+  </si>
+  <si>
+    <t>madelene.crooks@hotmail.com</t>
+  </si>
+  <si>
+    <t>josefina.weissnat@hotmail.com</t>
+  </si>
+  <si>
+    <t>lester.marvin@yahoo.com</t>
+  </si>
+  <si>
+    <t>blair.langosh@yahoo.com</t>
+  </si>
+  <si>
+    <t>ula20xmk8</t>
+  </si>
+  <si>
+    <t>giovanni.larkin@yahoo.com</t>
+  </si>
+  <si>
+    <t>xo3dhmd3vh</t>
+  </si>
+  <si>
+    <t>wynell.tremblay@gmail.com</t>
+  </si>
+  <si>
+    <t>wrww8cmt</t>
+  </si>
+  <si>
+    <t>winston.feil@gmail.com</t>
+  </si>
+  <si>
+    <t>yndn2uh4</t>
+  </si>
+  <si>
+    <t>shawn.wehner@hotmail.com</t>
+  </si>
+  <si>
+    <t>ldksakt9</t>
+  </si>
+  <si>
+    <t>ferdinand.tromp@gmail.com</t>
+  </si>
+  <si>
+    <t>rtm1s1fur</t>
+  </si>
+  <si>
+    <t>micha.mertz@hotmail.com</t>
+  </si>
+  <si>
+    <t>4uhbevikl0ndaz</t>
+  </si>
+  <si>
+    <t>blanche.gulgowski@yahoo.com</t>
+  </si>
+  <si>
+    <t>gzyycon69tdv8s</t>
+  </si>
+  <si>
+    <t>erlinda.padberg@hotmail.com</t>
+  </si>
+  <si>
+    <t>kgijjmw44</t>
+  </si>
+  <si>
+    <t>adolfo.terry@yahoo.com</t>
+  </si>
+  <si>
+    <t>los70114gy</t>
+  </si>
+  <si>
+    <t>mohammad.mosciski@yahoo.com</t>
+  </si>
+  <si>
+    <t>lyfrzaqjpl</t>
+  </si>
+  <si>
+    <t>ferdinand.kris@yahoo.com</t>
+  </si>
+  <si>
+    <t>xvgdmq69t9qbk</t>
+  </si>
+  <si>
+    <t>emory.towne@yahoo.com</t>
+  </si>
+  <si>
+    <t>p9yrtmidqhnt</t>
+  </si>
+  <si>
+    <t>dion.bruen@gmail.com</t>
+  </si>
+  <si>
+    <t>hqmpbjn84u</t>
+  </si>
+  <si>
+    <t>malisa.hammes@hotmail.com</t>
+  </si>
+  <si>
+    <t>nlfnial0</t>
+  </si>
+  <si>
+    <t>patrice.considine@yahoo.com</t>
+  </si>
+  <si>
+    <t>l6ednspb6k9w8xy</t>
+  </si>
+  <si>
+    <t>bonnie.crooks@yahoo.com</t>
+  </si>
+  <si>
+    <t>b0gvuqkzd</t>
+  </si>
+  <si>
+    <t>perry.brakus@gmail.com</t>
+  </si>
+  <si>
+    <t>7iuqcpkz0g6</t>
+  </si>
+  <si>
+    <t>domenica.beahan@yahoo.com</t>
+  </si>
+  <si>
+    <t>f2ilwmlnplyf53</t>
+  </si>
+  <si>
+    <t>antione.schowalter@gmail.com</t>
+  </si>
+  <si>
+    <t>54vg99my4f5l</t>
+  </si>
+  <si>
+    <t>joesph.ebert@gmail.com</t>
+  </si>
+  <si>
+    <t>x3ommy81y4qe26</t>
   </si>
 </sst>
 </file>
@@ -402,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="A6:B7"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -455,7 +590,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s" s="0">
         <v>8</v>
       </c>
@@ -463,7 +598,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s" s="0">
         <v>10</v>
       </c>
@@ -471,12 +606,212 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s" s="0">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s" s="0">
         <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="B32" t="s" s="0">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="B33" t="s" s="0">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>